<commit_message>
one more update to files for formatting
</commit_message>
<xml_diff>
--- a/data/social/S_1002.xlsx
+++ b/data/social/S_1002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/social/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763B0483-EB39-EC4A-AFAF-E08D53C3BF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789D3C0-076C-0544-8716-2D282C986BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI68"/>
+  <dimension ref="A1:AI72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1110,95 +1110,98 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1002</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>77.81</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>60.01</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>781033223</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="1">
-        <v>43811</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0.71615740740740741</v>
-      </c>
-      <c r="V2" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>21.21</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>6908</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>12</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>0.17666670000000001</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2">
         <v>0</v>
@@ -1214,95 +1217,98 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1002</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>77.81</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>60.01</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>781033223</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="1">
-        <v>43811</v>
-      </c>
-      <c r="U3" s="2">
-        <v>0.71615740740740741</v>
-      </c>
-      <c r="V3" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>9.91</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>1917</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>50</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>0.1628</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI3">
         <v>0</v>
@@ -1318,95 +1324,98 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1002</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>77.81</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>60.01</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>9</v>
-      </c>
-      <c r="L4" t="s">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>781033223</v>
-      </c>
-      <c r="P4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="1">
-        <v>43811</v>
-      </c>
-      <c r="U4" s="2">
-        <v>0.71615740740740741</v>
-      </c>
-      <c r="V4" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>19.95</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>1418</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <v>50</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>0.15964</v>
+        <v>0</v>
       </c>
       <c r="AF4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <v>0</v>
@@ -1422,98 +1431,101 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>32</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1002</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>77.81</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>60.01</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>9</v>
-      </c>
-      <c r="L5" t="s">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>781033223</v>
-      </c>
-      <c r="P5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="1">
-        <v>43811</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0.71615740740740741</v>
-      </c>
-      <c r="V5" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>22.47</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <v>993</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>88</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>0.17598</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI5">
-        <v>22.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
@@ -1581,19 +1593,19 @@
         <v>38</v>
       </c>
       <c r="W6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>12.42</v>
+        <v>21.21</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z6">
         <v>1</v>
       </c>
       <c r="AA6">
-        <v>1728</v>
+        <v>6908</v>
       </c>
       <c r="AB6">
         <v>12</v>
@@ -1605,16 +1617,16 @@
         <v>28</v>
       </c>
       <c r="AE6">
-        <v>0.15110000000000001</v>
+        <v>0.17666670000000001</v>
       </c>
       <c r="AF6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <v>1</v>
       </c>
       <c r="AH6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <v>0</v>
@@ -1685,43 +1697,43 @@
         <v>38</v>
       </c>
       <c r="W7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="X7">
-        <v>13.67</v>
+        <v>9.91</v>
       </c>
       <c r="Y7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7">
         <v>1</v>
       </c>
       <c r="AA7">
-        <v>1362</v>
+        <v>1917</v>
       </c>
       <c r="AB7">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD7" t="s">
         <v>28</v>
       </c>
       <c r="AE7">
-        <v>0.17132</v>
+        <v>0.1628</v>
       </c>
       <c r="AF7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AG7">
         <v>1</v>
       </c>
       <c r="AH7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AI7">
-        <v>13.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
@@ -1789,19 +1801,19 @@
         <v>38</v>
       </c>
       <c r="W8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X8">
-        <v>18.7</v>
+        <v>19.95</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <v>1</v>
       </c>
       <c r="AA8">
-        <v>2445</v>
+        <v>1418</v>
       </c>
       <c r="AB8">
         <v>50</v>
@@ -1813,16 +1825,16 @@
         <v>28</v>
       </c>
       <c r="AE8">
-        <v>0.1472</v>
+        <v>0.15964</v>
       </c>
       <c r="AF8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AG8">
         <v>1</v>
       </c>
       <c r="AH8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -1893,10 +1905,10 @@
         <v>38</v>
       </c>
       <c r="W9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X9">
-        <v>12.42</v>
+        <v>22.47</v>
       </c>
       <c r="Y9">
         <v>1</v>
@@ -1905,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="AA9">
-        <v>3495</v>
+        <v>993</v>
       </c>
       <c r="AB9">
         <v>88</v>
@@ -1917,19 +1929,19 @@
         <v>28</v>
       </c>
       <c r="AE9">
-        <v>0.17781</v>
+        <v>0.17598</v>
       </c>
       <c r="AF9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AG9">
         <v>1</v>
       </c>
       <c r="AH9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AI9">
-        <v>12.42</v>
+        <v>22.47</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
@@ -1997,10 +2009,10 @@
         <v>38</v>
       </c>
       <c r="W10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="X10">
-        <v>14.93</v>
+        <v>12.42</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -2009,31 +2021,31 @@
         <v>1</v>
       </c>
       <c r="AA10">
-        <v>1499</v>
+        <v>1728</v>
       </c>
       <c r="AB10">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="AC10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD10" t="s">
         <v>28</v>
       </c>
       <c r="AE10">
-        <v>0.14610000000000001</v>
+        <v>0.15110000000000001</v>
       </c>
       <c r="AF10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
       <c r="AH10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AI10">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -2101,22 +2113,22 @@
         <v>38</v>
       </c>
       <c r="W11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="X11">
-        <v>17.440000000000001</v>
+        <v>13.67</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>2573</v>
+        <v>1362</v>
       </c>
       <c r="AB11">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="AC11" t="s">
         <v>40</v>
@@ -2125,19 +2137,19 @@
         <v>28</v>
       </c>
       <c r="AE11">
-        <v>0.14499999999999999</v>
+        <v>0.17132</v>
       </c>
       <c r="AF11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AG11">
         <v>1</v>
       </c>
       <c r="AH11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AI11">
-        <v>7</v>
+        <v>13.67</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
@@ -2205,19 +2217,19 @@
         <v>38</v>
       </c>
       <c r="W12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="X12">
-        <v>27.49</v>
+        <v>18.7</v>
       </c>
       <c r="Y12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12">
         <v>1</v>
       </c>
       <c r="AA12">
-        <v>1357</v>
+        <v>2445</v>
       </c>
       <c r="AB12">
         <v>50</v>
@@ -2229,16 +2241,16 @@
         <v>28</v>
       </c>
       <c r="AE12">
-        <v>0.16864999999999999</v>
+        <v>0.1472</v>
       </c>
       <c r="AF12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AG12">
         <v>1</v>
       </c>
       <c r="AH12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AI12">
         <v>0</v>
@@ -2309,22 +2321,22 @@
         <v>38</v>
       </c>
       <c r="W13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="X13">
-        <v>16.190000000000001</v>
+        <v>12.42</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13">
         <v>1</v>
       </c>
       <c r="AA13">
-        <v>1419</v>
+        <v>3495</v>
       </c>
       <c r="AB13">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC13" t="s">
         <v>40</v>
@@ -2333,19 +2345,19 @@
         <v>28</v>
       </c>
       <c r="AE13">
-        <v>0.1622333</v>
+        <v>0.17781</v>
       </c>
       <c r="AF13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AG13">
         <v>1</v>
       </c>
       <c r="AH13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AI13">
-        <v>7</v>
+        <v>12.42</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
@@ -2413,7 +2425,7 @@
         <v>38</v>
       </c>
       <c r="W14">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="X14">
         <v>14.93</v>
@@ -2425,31 +2437,31 @@
         <v>1</v>
       </c>
       <c r="AA14">
-        <v>1061</v>
+        <v>1499</v>
       </c>
       <c r="AB14">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD14" t="s">
         <v>28</v>
       </c>
       <c r="AE14">
-        <v>0.15446670000000001</v>
+        <v>0.14610000000000001</v>
       </c>
       <c r="AF14">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AG14">
         <v>1</v>
       </c>
       <c r="AH14">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AI14">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
@@ -2517,10 +2529,10 @@
         <v>38</v>
       </c>
       <c r="W15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="X15">
-        <v>9.91</v>
+        <v>17.440000000000001</v>
       </c>
       <c r="Y15">
         <v>0</v>
@@ -2529,10 +2541,10 @@
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>4213</v>
+        <v>2573</v>
       </c>
       <c r="AB15">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC15" t="s">
         <v>40</v>
@@ -2541,16 +2553,16 @@
         <v>28</v>
       </c>
       <c r="AE15">
-        <v>0.14166670000000001</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="AF15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AG15">
         <v>1</v>
       </c>
       <c r="AH15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AI15">
         <v>7</v>
@@ -2621,10 +2633,10 @@
         <v>38</v>
       </c>
       <c r="W16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="X16">
-        <v>21.21</v>
+        <v>27.49</v>
       </c>
       <c r="Y16">
         <v>1</v>
@@ -2633,10 +2645,10 @@
         <v>1</v>
       </c>
       <c r="AA16">
-        <v>1424</v>
+        <v>1357</v>
       </c>
       <c r="AB16">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC16" t="s">
         <v>39</v>
@@ -2645,16 +2657,16 @@
         <v>28</v>
       </c>
       <c r="AE16">
-        <v>0.16814999999999999</v>
+        <v>0.16864999999999999</v>
       </c>
       <c r="AF16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AG16">
         <v>1</v>
       </c>
       <c r="AH16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AI16">
         <v>0</v>
@@ -2725,10 +2737,10 @@
         <v>38</v>
       </c>
       <c r="W17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="X17">
-        <v>8.65</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="Y17">
         <v>0</v>
@@ -2737,31 +2749,31 @@
         <v>1</v>
       </c>
       <c r="AA17">
-        <v>1348</v>
+        <v>1419</v>
       </c>
       <c r="AB17">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD17" t="s">
         <v>28</v>
       </c>
       <c r="AE17">
-        <v>0.14499999999999999</v>
+        <v>0.1622333</v>
       </c>
       <c r="AF17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AG17">
         <v>1</v>
       </c>
       <c r="AH17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI17">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.2">
@@ -2829,43 +2841,43 @@
         <v>38</v>
       </c>
       <c r="W18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="X18">
-        <v>24.98</v>
+        <v>14.93</v>
       </c>
       <c r="Y18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z18">
         <v>1</v>
       </c>
       <c r="AA18">
-        <v>1565</v>
+        <v>1061</v>
       </c>
       <c r="AB18">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD18" t="s">
         <v>28</v>
       </c>
       <c r="AE18">
-        <v>0.16780999999999999</v>
+        <v>0.15446670000000001</v>
       </c>
       <c r="AF18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AG18">
         <v>1</v>
       </c>
       <c r="AH18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AI18">
-        <v>24.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
@@ -2933,10 +2945,10 @@
         <v>38</v>
       </c>
       <c r="W19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="X19">
-        <v>16.190000000000001</v>
+        <v>9.91</v>
       </c>
       <c r="Y19">
         <v>0</v>
@@ -2945,31 +2957,31 @@
         <v>1</v>
       </c>
       <c r="AA19">
-        <v>1030</v>
+        <v>4213</v>
       </c>
       <c r="AB19">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="AC19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD19" t="s">
         <v>28</v>
       </c>
       <c r="AE19">
-        <v>0.15723329999999999</v>
+        <v>0.14166670000000001</v>
       </c>
       <c r="AF19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AG19">
         <v>1</v>
       </c>
       <c r="AH19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AI19">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
@@ -3037,10 +3049,10 @@
         <v>38</v>
       </c>
       <c r="W20">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="X20">
-        <v>28.74</v>
+        <v>21.21</v>
       </c>
       <c r="Y20">
         <v>1</v>
@@ -3049,31 +3061,31 @@
         <v>1</v>
       </c>
       <c r="AA20">
-        <v>1876</v>
+        <v>1424</v>
       </c>
       <c r="AB20">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD20" t="s">
         <v>28</v>
       </c>
       <c r="AE20">
-        <v>0.17881</v>
+        <v>0.16814999999999999</v>
       </c>
       <c r="AF20">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AG20">
         <v>1</v>
       </c>
       <c r="AH20">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AI20">
-        <v>28.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
@@ -3141,10 +3153,10 @@
         <v>38</v>
       </c>
       <c r="W21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="X21">
-        <v>28.74</v>
+        <v>8.65</v>
       </c>
       <c r="Y21">
         <v>0</v>
@@ -3153,7 +3165,7 @@
         <v>1</v>
       </c>
       <c r="AA21">
-        <v>2765</v>
+        <v>1348</v>
       </c>
       <c r="AB21">
         <v>12</v>
@@ -3165,16 +3177,16 @@
         <v>28</v>
       </c>
       <c r="AE21">
-        <v>0.15053330000000001</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="AF21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AG21">
         <v>1</v>
       </c>
       <c r="AH21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AI21">
         <v>0</v>
@@ -3245,10 +3257,10 @@
         <v>38</v>
       </c>
       <c r="W22">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="X22">
-        <v>17.440000000000001</v>
+        <v>24.98</v>
       </c>
       <c r="Y22">
         <v>1</v>
@@ -3257,10 +3269,10 @@
         <v>1</v>
       </c>
       <c r="AA22">
-        <v>1910</v>
+        <v>1565</v>
       </c>
       <c r="AB22">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC22" t="s">
         <v>40</v>
@@ -3269,19 +3281,19 @@
         <v>28</v>
       </c>
       <c r="AE22">
-        <v>0.17881</v>
+        <v>0.16780999999999999</v>
       </c>
       <c r="AF22">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AG22">
         <v>1</v>
       </c>
       <c r="AH22">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AI22">
-        <v>17.440000000000001</v>
+        <v>24.98</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
@@ -3349,10 +3361,10 @@
         <v>38</v>
       </c>
       <c r="W23">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="X23">
-        <v>27.49</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -3361,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="AA23">
-        <v>1485</v>
+        <v>1030</v>
       </c>
       <c r="AB23">
         <v>12</v>
@@ -3373,16 +3385,16 @@
         <v>28</v>
       </c>
       <c r="AE23">
-        <v>0.15279999999999999</v>
+        <v>0.15723329999999999</v>
       </c>
       <c r="AF23">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AG23">
         <v>1</v>
       </c>
       <c r="AH23">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AI23">
         <v>0</v>
@@ -3453,43 +3465,43 @@
         <v>38</v>
       </c>
       <c r="W24">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="X24">
-        <v>22.47</v>
+        <v>28.74</v>
       </c>
       <c r="Y24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24">
         <v>1</v>
       </c>
       <c r="AA24">
-        <v>1319</v>
+        <v>1876</v>
       </c>
       <c r="AB24">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD24" t="s">
         <v>28</v>
       </c>
       <c r="AE24">
-        <v>0.15053330000000001</v>
+        <v>0.17881</v>
       </c>
       <c r="AF24">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AG24">
         <v>1</v>
       </c>
       <c r="AH24">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AI24">
-        <v>0</v>
+        <v>28.74</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
@@ -3557,43 +3569,43 @@
         <v>38</v>
       </c>
       <c r="W25">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="X25">
         <v>28.74</v>
       </c>
       <c r="Y25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z25">
         <v>1</v>
       </c>
       <c r="AA25">
-        <v>1594</v>
+        <v>2765</v>
       </c>
       <c r="AB25">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD25" t="s">
         <v>28</v>
       </c>
       <c r="AE25">
-        <v>0.17630999999999999</v>
+        <v>0.15053330000000001</v>
       </c>
       <c r="AF25">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AG25">
         <v>1</v>
       </c>
       <c r="AH25">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AI25">
-        <v>28.74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
@@ -3661,10 +3673,10 @@
         <v>38</v>
       </c>
       <c r="W26">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X26">
-        <v>18.7</v>
+        <v>17.440000000000001</v>
       </c>
       <c r="Y26">
         <v>1</v>
@@ -3673,10 +3685,10 @@
         <v>1</v>
       </c>
       <c r="AA26">
-        <v>1608</v>
+        <v>1910</v>
       </c>
       <c r="AB26">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC26" t="s">
         <v>40</v>
@@ -3685,19 +3697,19 @@
         <v>28</v>
       </c>
       <c r="AE26">
-        <v>0.17763999999999999</v>
+        <v>0.17881</v>
       </c>
       <c r="AF26">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AG26">
         <v>1</v>
       </c>
       <c r="AH26">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AI26">
-        <v>18.7</v>
+        <v>17.440000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
@@ -3765,10 +3777,10 @@
         <v>38</v>
       </c>
       <c r="W27">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="X27">
-        <v>23.72</v>
+        <v>27.49</v>
       </c>
       <c r="Y27">
         <v>0</v>
@@ -3777,10 +3789,10 @@
         <v>1</v>
       </c>
       <c r="AA27">
-        <v>2856</v>
+        <v>1485</v>
       </c>
       <c r="AB27">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="AC27" t="s">
         <v>39</v>
@@ -3789,16 +3801,16 @@
         <v>28</v>
       </c>
       <c r="AE27">
-        <v>0.15333330000000001</v>
+        <v>0.15279999999999999</v>
       </c>
       <c r="AF27">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AG27">
         <v>1</v>
       </c>
       <c r="AH27">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AI27">
         <v>0</v>
@@ -3869,43 +3881,43 @@
         <v>38</v>
       </c>
       <c r="W28">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="X28">
-        <v>17.440000000000001</v>
+        <v>22.47</v>
       </c>
       <c r="Y28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z28">
         <v>1</v>
       </c>
       <c r="AA28">
-        <v>1555</v>
+        <v>1319</v>
       </c>
       <c r="AB28">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD28" t="s">
         <v>28</v>
       </c>
       <c r="AE28">
-        <v>0.18348</v>
+        <v>0.15053330000000001</v>
       </c>
       <c r="AF28">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AG28">
         <v>1</v>
       </c>
       <c r="AH28">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AI28">
-        <v>17.440000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
@@ -3973,43 +3985,43 @@
         <v>38</v>
       </c>
       <c r="W29">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="X29">
-        <v>26.23</v>
+        <v>28.74</v>
       </c>
       <c r="Y29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z29">
         <v>1</v>
       </c>
       <c r="AA29">
-        <v>1022</v>
+        <v>1594</v>
       </c>
       <c r="AB29">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD29" t="s">
         <v>28</v>
       </c>
       <c r="AE29">
-        <v>0.15609999999999999</v>
+        <v>0.17630999999999999</v>
       </c>
       <c r="AF29">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AG29">
         <v>1</v>
       </c>
       <c r="AH29">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AI29">
-        <v>0</v>
+        <v>28.74</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
@@ -4077,22 +4089,22 @@
         <v>38</v>
       </c>
       <c r="W30">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="X30">
-        <v>12.42</v>
+        <v>18.7</v>
       </c>
       <c r="Y30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z30">
         <v>1</v>
       </c>
       <c r="AA30">
-        <v>2182</v>
+        <v>1608</v>
       </c>
       <c r="AB30">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC30" t="s">
         <v>40</v>
@@ -4101,19 +4113,19 @@
         <v>28</v>
       </c>
       <c r="AE30">
-        <v>0.15390000000000001</v>
+        <v>0.17763999999999999</v>
       </c>
       <c r="AF30">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="AG30">
         <v>1</v>
       </c>
       <c r="AH30">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="AI30">
-        <v>7</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
@@ -4181,10 +4193,10 @@
         <v>38</v>
       </c>
       <c r="W31">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="X31">
-        <v>9.91</v>
+        <v>23.72</v>
       </c>
       <c r="Y31">
         <v>0</v>
@@ -4193,10 +4205,10 @@
         <v>1</v>
       </c>
       <c r="AA31">
-        <v>1019</v>
+        <v>2856</v>
       </c>
       <c r="AB31">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC31" t="s">
         <v>39</v>
@@ -4205,16 +4217,16 @@
         <v>28</v>
       </c>
       <c r="AE31">
-        <v>0.1511333</v>
+        <v>0.15333330000000001</v>
       </c>
       <c r="AF31">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="AG31">
         <v>1</v>
       </c>
       <c r="AH31">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="AI31">
         <v>0</v>
@@ -4285,43 +4297,43 @@
         <v>38</v>
       </c>
       <c r="W32">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="X32">
-        <v>21.21</v>
+        <v>17.440000000000001</v>
       </c>
       <c r="Y32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32">
         <v>1</v>
       </c>
       <c r="AA32">
-        <v>1714</v>
+        <v>1555</v>
       </c>
       <c r="AB32">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD32" t="s">
         <v>28</v>
       </c>
       <c r="AE32">
-        <v>0.16</v>
+        <v>0.18348</v>
       </c>
       <c r="AF32">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AG32">
         <v>1</v>
       </c>
       <c r="AH32">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AI32">
-        <v>0</v>
+        <v>17.440000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
@@ -4389,43 +4401,43 @@
         <v>38</v>
       </c>
       <c r="W33">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="X33">
-        <v>23.72</v>
+        <v>26.23</v>
       </c>
       <c r="Y33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z33">
         <v>1</v>
       </c>
       <c r="AA33">
-        <v>1546</v>
+        <v>1022</v>
       </c>
       <c r="AB33">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD33" t="s">
         <v>28</v>
       </c>
       <c r="AE33">
-        <v>0.17680999999999999</v>
+        <v>0.15609999999999999</v>
       </c>
       <c r="AF33">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AG33">
         <v>1</v>
       </c>
       <c r="AH33">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AI33">
-        <v>23.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.2">
@@ -4493,10 +4505,10 @@
         <v>38</v>
       </c>
       <c r="W34">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="X34">
-        <v>22.47</v>
+        <v>12.42</v>
       </c>
       <c r="Y34">
         <v>0</v>
@@ -4505,13 +4517,13 @@
         <v>1</v>
       </c>
       <c r="AA34">
-        <v>1992</v>
+        <v>2182</v>
       </c>
       <c r="AB34">
         <v>50</v>
       </c>
       <c r="AC34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD34" t="s">
         <v>28</v>
@@ -4520,16 +4532,16 @@
         <v>0.15390000000000001</v>
       </c>
       <c r="AF34">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AG34">
         <v>1</v>
       </c>
       <c r="AH34">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AI34">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
@@ -4597,10 +4609,10 @@
         <v>38</v>
       </c>
       <c r="W35">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="X35">
-        <v>8.65</v>
+        <v>9.91</v>
       </c>
       <c r="Y35">
         <v>0</v>
@@ -4609,31 +4621,31 @@
         <v>1</v>
       </c>
       <c r="AA35">
-        <v>2860</v>
+        <v>1019</v>
       </c>
       <c r="AB35">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD35" t="s">
         <v>28</v>
       </c>
       <c r="AE35">
-        <v>0.16109999999999999</v>
+        <v>0.1511333</v>
       </c>
       <c r="AF35">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AG35">
         <v>1</v>
       </c>
       <c r="AH35">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AI35">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
@@ -4701,10 +4713,10 @@
         <v>38</v>
       </c>
       <c r="W36">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="X36">
-        <v>24.98</v>
+        <v>21.21</v>
       </c>
       <c r="Y36">
         <v>0</v>
@@ -4713,10 +4725,10 @@
         <v>1</v>
       </c>
       <c r="AA36">
-        <v>1389</v>
+        <v>1714</v>
       </c>
       <c r="AB36">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC36" t="s">
         <v>39</v>
@@ -4725,16 +4737,16 @@
         <v>28</v>
       </c>
       <c r="AE36">
-        <v>0.1538667</v>
+        <v>0.16</v>
       </c>
       <c r="AF36">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AG36">
         <v>1</v>
       </c>
       <c r="AH36">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AI36">
         <v>0</v>
@@ -4805,43 +4817,43 @@
         <v>38</v>
       </c>
       <c r="W37">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="X37">
-        <v>26.23</v>
+        <v>23.72</v>
       </c>
       <c r="Y37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z37">
         <v>1</v>
       </c>
       <c r="AA37">
-        <v>1274</v>
+        <v>1546</v>
       </c>
       <c r="AB37">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="AC37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD37" t="s">
         <v>28</v>
       </c>
       <c r="AE37">
-        <v>0.15666669999999999</v>
+        <v>0.17680999999999999</v>
       </c>
       <c r="AF37">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AG37">
         <v>1</v>
       </c>
       <c r="AH37">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AI37">
-        <v>0</v>
+        <v>23.72</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
@@ -4909,43 +4921,43 @@
         <v>38</v>
       </c>
       <c r="W38">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="X38">
-        <v>26.23</v>
+        <v>22.47</v>
       </c>
       <c r="Y38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z38">
         <v>1</v>
       </c>
       <c r="AA38">
-        <v>1287</v>
+        <v>1992</v>
       </c>
       <c r="AB38">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD38" t="s">
         <v>28</v>
       </c>
       <c r="AE38">
-        <v>0.17297999999999999</v>
+        <v>0.15390000000000001</v>
       </c>
       <c r="AF38">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AG38">
         <v>1</v>
       </c>
       <c r="AH38">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AI38">
-        <v>26.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
@@ -5013,19 +5025,19 @@
         <v>38</v>
       </c>
       <c r="W39">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="X39">
-        <v>14.93</v>
+        <v>8.65</v>
       </c>
       <c r="Y39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z39">
         <v>1</v>
       </c>
       <c r="AA39">
-        <v>1319</v>
+        <v>2860</v>
       </c>
       <c r="AB39">
         <v>88</v>
@@ -5037,19 +5049,19 @@
         <v>28</v>
       </c>
       <c r="AE39">
-        <v>0.17998</v>
+        <v>0.16109999999999999</v>
       </c>
       <c r="AF39">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AG39">
         <v>1</v>
       </c>
       <c r="AH39">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AI39">
-        <v>14.93</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
@@ -5117,7 +5129,7 @@
         <v>38</v>
       </c>
       <c r="W40">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="X40">
         <v>24.98</v>
@@ -5129,31 +5141,31 @@
         <v>1</v>
       </c>
       <c r="AA40">
-        <v>1489</v>
+        <v>1389</v>
       </c>
       <c r="AB40">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="AC40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD40" t="s">
         <v>28</v>
       </c>
       <c r="AE40">
-        <v>0.1555667</v>
+        <v>0.1538667</v>
       </c>
       <c r="AF40">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AG40">
         <v>1</v>
       </c>
       <c r="AH40">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AI40">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
@@ -5221,22 +5233,22 @@
         <v>38</v>
       </c>
       <c r="W41">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="X41">
-        <v>11.16</v>
+        <v>26.23</v>
       </c>
       <c r="Y41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z41">
         <v>1</v>
       </c>
       <c r="AA41">
-        <v>2095</v>
+        <v>1274</v>
       </c>
       <c r="AB41">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC41" t="s">
         <v>39</v>
@@ -5245,16 +5257,16 @@
         <v>28</v>
       </c>
       <c r="AE41">
-        <v>0.18581</v>
+        <v>0.15666669999999999</v>
       </c>
       <c r="AF41">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AG41">
         <v>1</v>
       </c>
       <c r="AH41">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AI41">
         <v>0</v>
@@ -5325,43 +5337,43 @@
         <v>38</v>
       </c>
       <c r="W42">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="X42">
-        <v>19.95</v>
+        <v>26.23</v>
       </c>
       <c r="Y42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z42">
         <v>1</v>
       </c>
       <c r="AA42">
-        <v>1306</v>
+        <v>1287</v>
       </c>
       <c r="AB42">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="AC42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD42" t="s">
         <v>28</v>
       </c>
       <c r="AE42">
-        <v>0.15390000000000001</v>
+        <v>0.17297999999999999</v>
       </c>
       <c r="AF42">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AG42">
         <v>1</v>
       </c>
       <c r="AH42">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AI42">
-        <v>0</v>
+        <v>26.23</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
@@ -5429,43 +5441,43 @@
         <v>38</v>
       </c>
       <c r="W43">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="X43">
-        <v>18.7</v>
+        <v>14.93</v>
       </c>
       <c r="Y43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z43">
         <v>1</v>
       </c>
       <c r="AA43">
-        <v>1291</v>
+        <v>1319</v>
       </c>
       <c r="AB43">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="AC43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD43" t="s">
         <v>28</v>
       </c>
       <c r="AE43">
-        <v>0.1555667</v>
+        <v>0.17998</v>
       </c>
       <c r="AF43">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AG43">
         <v>1</v>
       </c>
       <c r="AH43">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AI43">
-        <v>0</v>
+        <v>14.93</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.2">
@@ -5533,10 +5545,10 @@
         <v>38</v>
       </c>
       <c r="W44">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="X44">
-        <v>8.65</v>
+        <v>24.98</v>
       </c>
       <c r="Y44">
         <v>0</v>
@@ -5545,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="AA44">
-        <v>1121</v>
+        <v>1489</v>
       </c>
       <c r="AB44">
         <v>50</v>
@@ -5557,16 +5569,16 @@
         <v>28</v>
       </c>
       <c r="AE44">
-        <v>0.1616667</v>
+        <v>0.1555667</v>
       </c>
       <c r="AF44">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AG44">
         <v>1</v>
       </c>
       <c r="AH44">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AI44">
         <v>7</v>
@@ -5637,22 +5649,22 @@
         <v>38</v>
       </c>
       <c r="W45">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="X45">
-        <v>13.67</v>
+        <v>11.16</v>
       </c>
       <c r="Y45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z45">
         <v>1</v>
       </c>
       <c r="AA45">
-        <v>1607</v>
+        <v>2095</v>
       </c>
       <c r="AB45">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC45" t="s">
         <v>39</v>
@@ -5661,16 +5673,16 @@
         <v>28</v>
       </c>
       <c r="AE45">
-        <v>0.16113330000000001</v>
+        <v>0.18581</v>
       </c>
       <c r="AF45">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AG45">
         <v>1</v>
       </c>
       <c r="AH45">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AI45">
         <v>0</v>
@@ -5741,10 +5753,10 @@
         <v>38</v>
       </c>
       <c r="W46">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="X46">
-        <v>11.16</v>
+        <v>19.95</v>
       </c>
       <c r="Y46">
         <v>0</v>
@@ -5753,31 +5765,31 @@
         <v>1</v>
       </c>
       <c r="AA46">
-        <v>2362</v>
+        <v>1306</v>
       </c>
       <c r="AB46">
         <v>12</v>
       </c>
       <c r="AC46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD46" t="s">
         <v>28</v>
       </c>
       <c r="AE46">
-        <v>0.14946670000000001</v>
+        <v>0.15390000000000001</v>
       </c>
       <c r="AF46">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AG46">
         <v>1</v>
       </c>
       <c r="AH46">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AI46">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.2">
@@ -5845,43 +5857,43 @@
         <v>38</v>
       </c>
       <c r="W47">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="X47">
-        <v>19.95</v>
+        <v>18.7</v>
       </c>
       <c r="Y47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z47">
         <v>1</v>
       </c>
       <c r="AA47">
-        <v>2245</v>
+        <v>1291</v>
       </c>
       <c r="AB47">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD47" t="s">
         <v>28</v>
       </c>
       <c r="AE47">
-        <v>0.17247999999999999</v>
+        <v>0.1555667</v>
       </c>
       <c r="AF47">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AG47">
         <v>1</v>
       </c>
       <c r="AH47">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AI47">
-        <v>19.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">
@@ -5949,22 +5961,22 @@
         <v>38</v>
       </c>
       <c r="W48">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="X48">
-        <v>16.190000000000001</v>
+        <v>8.65</v>
       </c>
       <c r="Y48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z48">
         <v>1</v>
       </c>
       <c r="AA48">
-        <v>1504</v>
+        <v>1121</v>
       </c>
       <c r="AB48">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC48" t="s">
         <v>40</v>
@@ -5973,19 +5985,19 @@
         <v>28</v>
       </c>
       <c r="AE48">
-        <v>0.17698</v>
+        <v>0.1616667</v>
       </c>
       <c r="AF48">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AG48">
         <v>1</v>
       </c>
       <c r="AH48">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AI48">
-        <v>16.190000000000001</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
@@ -6053,10 +6065,10 @@
         <v>38</v>
       </c>
       <c r="W49">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="X49">
-        <v>23.72</v>
+        <v>13.67</v>
       </c>
       <c r="Y49">
         <v>0</v>
@@ -6065,10 +6077,10 @@
         <v>1</v>
       </c>
       <c r="AA49">
-        <v>1407</v>
+        <v>1607</v>
       </c>
       <c r="AB49">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC49" t="s">
         <v>39</v>
@@ -6077,16 +6089,16 @@
         <v>28</v>
       </c>
       <c r="AE49">
-        <v>0.1555667</v>
+        <v>0.16113330000000001</v>
       </c>
       <c r="AF49">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AG49">
         <v>1</v>
       </c>
       <c r="AH49">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AI49">
         <v>0</v>
@@ -6157,22 +6169,22 @@
         <v>38</v>
       </c>
       <c r="W50">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="X50">
-        <v>27.49</v>
+        <v>11.16</v>
       </c>
       <c r="Y50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z50">
         <v>1</v>
       </c>
       <c r="AA50">
-        <v>2505</v>
+        <v>2362</v>
       </c>
       <c r="AB50">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC50" t="s">
         <v>40</v>
@@ -6181,19 +6193,19 @@
         <v>28</v>
       </c>
       <c r="AE50">
-        <v>0.16897999999999999</v>
+        <v>0.14946670000000001</v>
       </c>
       <c r="AF50">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AG50">
         <v>1</v>
       </c>
       <c r="AH50">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AI50">
-        <v>27.49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.2">
@@ -6261,43 +6273,43 @@
         <v>38</v>
       </c>
       <c r="W51">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="X51">
-        <v>13.67</v>
+        <v>19.95</v>
       </c>
       <c r="Y51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z51">
         <v>1</v>
       </c>
       <c r="AA51">
-        <v>1568</v>
+        <v>2245</v>
       </c>
       <c r="AB51">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="AC51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD51" t="s">
         <v>28</v>
       </c>
       <c r="AE51">
-        <v>0.15946669999999999</v>
+        <v>0.17247999999999999</v>
       </c>
       <c r="AF51">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AG51">
         <v>1</v>
       </c>
       <c r="AH51">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AI51">
-        <v>0</v>
+        <v>19.95</v>
       </c>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.2">
@@ -6365,22 +6377,22 @@
         <v>38</v>
       </c>
       <c r="W52">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="X52">
-        <v>11.16</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="Y52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z52">
         <v>1</v>
       </c>
       <c r="AA52">
-        <v>2423</v>
+        <v>1504</v>
       </c>
       <c r="AB52">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC52" t="s">
         <v>40</v>
@@ -6389,19 +6401,19 @@
         <v>28</v>
       </c>
       <c r="AE52">
-        <v>0.155</v>
+        <v>0.17698</v>
       </c>
       <c r="AF52">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="AG52">
         <v>1</v>
       </c>
       <c r="AH52">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="AI52">
-        <v>7</v>
+        <v>16.190000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
@@ -6469,10 +6481,10 @@
         <v>38</v>
       </c>
       <c r="W53">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="X53">
-        <v>18.07</v>
+        <v>23.72</v>
       </c>
       <c r="Y53">
         <v>0</v>
@@ -6481,7 +6493,7 @@
         <v>1</v>
       </c>
       <c r="AA53">
-        <v>1649</v>
+        <v>1407</v>
       </c>
       <c r="AB53">
         <v>12</v>
@@ -6493,16 +6505,16 @@
         <v>28</v>
       </c>
       <c r="AE53">
-        <v>0.16109999999999999</v>
+        <v>0.1555667</v>
       </c>
       <c r="AF53">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AG53">
         <v>1</v>
       </c>
       <c r="AH53">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AI53">
         <v>0</v>
@@ -6573,10 +6585,10 @@
         <v>38</v>
       </c>
       <c r="W54">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="X54">
-        <v>24.35</v>
+        <v>27.49</v>
       </c>
       <c r="Y54">
         <v>1</v>
@@ -6585,31 +6597,31 @@
         <v>1</v>
       </c>
       <c r="AA54">
-        <v>1211</v>
+        <v>2505</v>
       </c>
       <c r="AB54">
         <v>88</v>
       </c>
       <c r="AC54" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD54" t="s">
         <v>28</v>
       </c>
       <c r="AE54">
-        <v>0.17280999999999999</v>
+        <v>0.16897999999999999</v>
       </c>
       <c r="AF54">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AG54">
         <v>1</v>
       </c>
       <c r="AH54">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AI54">
-        <v>0</v>
+        <v>27.49</v>
       </c>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
@@ -6677,22 +6689,22 @@
         <v>38</v>
       </c>
       <c r="W55">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="X55">
-        <v>26.86</v>
+        <v>13.67</v>
       </c>
       <c r="Y55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z55">
         <v>1</v>
       </c>
       <c r="AA55">
-        <v>2373</v>
+        <v>1568</v>
       </c>
       <c r="AB55">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="AC55" t="s">
         <v>39</v>
@@ -6701,16 +6713,16 @@
         <v>28</v>
       </c>
       <c r="AE55">
-        <v>0.18681</v>
+        <v>0.15946669999999999</v>
       </c>
       <c r="AF55">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AG55">
         <v>1</v>
       </c>
       <c r="AH55">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AI55">
         <v>0</v>
@@ -6781,22 +6793,22 @@
         <v>38</v>
       </c>
       <c r="W56">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="X56">
-        <v>29.37</v>
+        <v>11.16</v>
       </c>
       <c r="Y56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z56">
         <v>1</v>
       </c>
       <c r="AA56">
-        <v>1259</v>
+        <v>2423</v>
       </c>
       <c r="AB56">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC56" t="s">
         <v>40</v>
@@ -6805,19 +6817,19 @@
         <v>28</v>
       </c>
       <c r="AE56">
-        <v>0.18314</v>
+        <v>0.155</v>
       </c>
       <c r="AF56">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AG56">
         <v>1</v>
       </c>
       <c r="AH56">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AI56">
-        <v>29.37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
@@ -6885,19 +6897,19 @@
         <v>38</v>
       </c>
       <c r="W57">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="X57">
-        <v>28.12</v>
+        <v>18.07</v>
       </c>
       <c r="Y57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z57">
         <v>1</v>
       </c>
       <c r="AA57">
-        <v>5754</v>
+        <v>1649</v>
       </c>
       <c r="AB57">
         <v>12</v>
@@ -6909,16 +6921,16 @@
         <v>28</v>
       </c>
       <c r="AE57">
-        <v>0.17898</v>
+        <v>0.16109999999999999</v>
       </c>
       <c r="AF57">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AG57">
         <v>1</v>
       </c>
       <c r="AH57">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AI57">
         <v>0</v>
@@ -6989,10 +7001,10 @@
         <v>38</v>
       </c>
       <c r="W58">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="X58">
-        <v>25.6</v>
+        <v>24.35</v>
       </c>
       <c r="Y58">
         <v>1</v>
@@ -7001,31 +7013,31 @@
         <v>1</v>
       </c>
       <c r="AA58">
-        <v>1222</v>
+        <v>1211</v>
       </c>
       <c r="AB58">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD58" t="s">
         <v>28</v>
       </c>
       <c r="AE58">
-        <v>0.19497</v>
+        <v>0.17280999999999999</v>
       </c>
       <c r="AF58">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG58">
         <v>1</v>
       </c>
       <c r="AH58">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AI58">
-        <v>25.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.2">
@@ -7093,22 +7105,22 @@
         <v>38</v>
       </c>
       <c r="W59">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="X59">
-        <v>25.6</v>
+        <v>26.86</v>
       </c>
       <c r="Y59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z59">
         <v>1</v>
       </c>
       <c r="AA59">
-        <v>1368</v>
+        <v>2373</v>
       </c>
       <c r="AB59">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AC59" t="s">
         <v>39</v>
@@ -7117,16 +7129,16 @@
         <v>28</v>
       </c>
       <c r="AE59">
-        <v>0.15333330000000001</v>
+        <v>0.18681</v>
       </c>
       <c r="AF59">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG59">
         <v>1</v>
       </c>
       <c r="AH59">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AI59">
         <v>0</v>
@@ -7197,10 +7209,10 @@
         <v>38</v>
       </c>
       <c r="W60">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="X60">
-        <v>28.12</v>
+        <v>29.37</v>
       </c>
       <c r="Y60">
         <v>1</v>
@@ -7209,7 +7221,7 @@
         <v>1</v>
       </c>
       <c r="AA60">
-        <v>1398</v>
+        <v>1259</v>
       </c>
       <c r="AB60">
         <v>88</v>
@@ -7221,19 +7233,19 @@
         <v>28</v>
       </c>
       <c r="AE60">
-        <v>0.18748000000000001</v>
+        <v>0.18314</v>
       </c>
       <c r="AF60">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AG60">
         <v>1</v>
       </c>
       <c r="AH60">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AI60">
-        <v>28.12</v>
+        <v>29.37</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.2">
@@ -7301,22 +7313,22 @@
         <v>38</v>
       </c>
       <c r="W61">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="X61">
-        <v>19.329999999999998</v>
+        <v>28.12</v>
       </c>
       <c r="Y61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z61">
         <v>1</v>
       </c>
       <c r="AA61">
-        <v>1391</v>
+        <v>5754</v>
       </c>
       <c r="AB61">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="AC61" t="s">
         <v>39</v>
@@ -7325,16 +7337,16 @@
         <v>28</v>
       </c>
       <c r="AE61">
-        <v>0.1555667</v>
+        <v>0.17898</v>
       </c>
       <c r="AF61">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AG61">
         <v>1</v>
       </c>
       <c r="AH61">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AI61">
         <v>0</v>
@@ -7405,10 +7417,10 @@
         <v>38</v>
       </c>
       <c r="W62">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="X62">
-        <v>10.53</v>
+        <v>25.6</v>
       </c>
       <c r="Y62">
         <v>1</v>
@@ -7417,10 +7429,10 @@
         <v>1</v>
       </c>
       <c r="AA62">
-        <v>2306</v>
+        <v>1222</v>
       </c>
       <c r="AB62">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC62" t="s">
         <v>40</v>
@@ -7429,19 +7441,19 @@
         <v>28</v>
       </c>
       <c r="AE62">
-        <v>0.19697000000000001</v>
+        <v>0.19497</v>
       </c>
       <c r="AF62">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AG62">
         <v>1</v>
       </c>
       <c r="AH62">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AI62">
-        <v>10.53</v>
+        <v>25.6</v>
       </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
@@ -7509,22 +7521,22 @@
         <v>38</v>
       </c>
       <c r="W63">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="X63">
-        <v>13.05</v>
+        <v>25.6</v>
       </c>
       <c r="Y63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z63">
         <v>1</v>
       </c>
       <c r="AA63">
-        <v>2096</v>
+        <v>1368</v>
       </c>
       <c r="AB63">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="AC63" t="s">
         <v>39</v>
@@ -7533,16 +7545,16 @@
         <v>28</v>
       </c>
       <c r="AE63">
-        <v>0.18648000000000001</v>
+        <v>0.15333330000000001</v>
       </c>
       <c r="AF63">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AG63">
         <v>1</v>
       </c>
       <c r="AH63">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AI63">
         <v>0</v>
@@ -7613,10 +7625,10 @@
         <v>38</v>
       </c>
       <c r="W64">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="X64">
-        <v>29.37</v>
+        <v>28.12</v>
       </c>
       <c r="Y64">
         <v>1</v>
@@ -7625,31 +7637,31 @@
         <v>1</v>
       </c>
       <c r="AA64">
-        <v>1778</v>
+        <v>1398</v>
       </c>
       <c r="AB64">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD64" t="s">
         <v>28</v>
       </c>
       <c r="AE64">
-        <v>0.18581</v>
+        <v>0.18748000000000001</v>
       </c>
       <c r="AF64">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AG64">
         <v>1</v>
       </c>
       <c r="AH64">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AI64">
-        <v>0</v>
+        <v>28.12</v>
       </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.2">
@@ -7717,10 +7729,10 @@
         <v>38</v>
       </c>
       <c r="W65">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="X65">
-        <v>9.2799999999999994</v>
+        <v>19.329999999999998</v>
       </c>
       <c r="Y65">
         <v>0</v>
@@ -7729,31 +7741,31 @@
         <v>1</v>
       </c>
       <c r="AA65">
-        <v>1458</v>
+        <v>1391</v>
       </c>
       <c r="AB65">
         <v>50</v>
       </c>
       <c r="AC65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD65" t="s">
         <v>28</v>
       </c>
       <c r="AE65">
-        <v>0.15390000000000001</v>
+        <v>0.1555667</v>
       </c>
       <c r="AF65">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AG65">
         <v>1</v>
       </c>
       <c r="AH65">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AI65">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.2">
@@ -7821,22 +7833,22 @@
         <v>38</v>
       </c>
       <c r="W66">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="X66">
-        <v>13.05</v>
+        <v>10.53</v>
       </c>
       <c r="Y66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z66">
         <v>1</v>
       </c>
       <c r="AA66">
-        <v>988</v>
+        <v>2306</v>
       </c>
       <c r="AB66">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC66" t="s">
         <v>40</v>
@@ -7845,19 +7857,19 @@
         <v>28</v>
       </c>
       <c r="AE66">
-        <v>0.1505667</v>
+        <v>0.19697000000000001</v>
       </c>
       <c r="AF66">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AG66">
         <v>1</v>
       </c>
       <c r="AH66">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AI66">
-        <v>7</v>
+        <v>10.53</v>
       </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.2">
@@ -7925,43 +7937,43 @@
         <v>38</v>
       </c>
       <c r="W67">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X67">
-        <v>10.53</v>
+        <v>13.05</v>
       </c>
       <c r="Y67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z67">
         <v>1</v>
       </c>
       <c r="AA67">
-        <v>1060</v>
+        <v>2096</v>
       </c>
       <c r="AB67">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AC67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD67" t="s">
         <v>28</v>
       </c>
       <c r="AE67">
-        <v>0.14610000000000001</v>
+        <v>0.18648000000000001</v>
       </c>
       <c r="AF67">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AG67">
         <v>1</v>
       </c>
       <c r="AH67">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AI67">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.2">
@@ -8029,10 +8041,10 @@
         <v>38</v>
       </c>
       <c r="W68">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="X68">
-        <v>21.84</v>
+        <v>29.37</v>
       </c>
       <c r="Y68">
         <v>1</v>
@@ -8041,30 +8053,446 @@
         <v>1</v>
       </c>
       <c r="AA68">
-        <v>1591</v>
+        <v>1778</v>
       </c>
       <c r="AB68">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AC68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD68" t="s">
         <v>28</v>
       </c>
       <c r="AE68">
+        <v>0.18581</v>
+      </c>
+      <c r="AF68">
+        <v>63</v>
+      </c>
+      <c r="AG68">
+        <v>1</v>
+      </c>
+      <c r="AH68">
+        <v>63</v>
+      </c>
+      <c r="AI68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69">
+        <v>1002</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>77.81</v>
+      </c>
+      <c r="H69" t="s">
+        <v>33</v>
+      </c>
+      <c r="I69" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69">
+        <v>60.01</v>
+      </c>
+      <c r="K69">
+        <v>9</v>
+      </c>
+      <c r="L69" t="s">
+        <v>35</v>
+      </c>
+      <c r="M69">
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <v>7</v>
+      </c>
+      <c r="O69">
+        <v>781033223</v>
+      </c>
+      <c r="P69" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>37</v>
+      </c>
+      <c r="R69" t="s">
+        <v>37</v>
+      </c>
+      <c r="S69" s="1">
+        <v>43811</v>
+      </c>
+      <c r="U69" s="2">
+        <v>0.71615740740740741</v>
+      </c>
+      <c r="V69" t="s">
+        <v>38</v>
+      </c>
+      <c r="W69">
+        <v>64</v>
+      </c>
+      <c r="X69">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="Y69">
+        <v>0</v>
+      </c>
+      <c r="Z69">
+        <v>1</v>
+      </c>
+      <c r="AA69">
+        <v>1458</v>
+      </c>
+      <c r="AB69">
+        <v>50</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE69">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="AF69">
+        <v>64</v>
+      </c>
+      <c r="AG69">
+        <v>1</v>
+      </c>
+      <c r="AH69">
+        <v>64</v>
+      </c>
+      <c r="AI69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70">
+        <v>1002</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>77.81</v>
+      </c>
+      <c r="H70" t="s">
+        <v>33</v>
+      </c>
+      <c r="I70" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70">
+        <v>60.01</v>
+      </c>
+      <c r="K70">
+        <v>9</v>
+      </c>
+      <c r="L70" t="s">
+        <v>35</v>
+      </c>
+      <c r="M70">
+        <v>1</v>
+      </c>
+      <c r="N70">
+        <v>7</v>
+      </c>
+      <c r="O70">
+        <v>781033223</v>
+      </c>
+      <c r="P70" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>37</v>
+      </c>
+      <c r="R70" t="s">
+        <v>37</v>
+      </c>
+      <c r="S70" s="1">
+        <v>43811</v>
+      </c>
+      <c r="U70" s="2">
+        <v>0.71615740740740741</v>
+      </c>
+      <c r="V70" t="s">
+        <v>38</v>
+      </c>
+      <c r="W70">
+        <v>65</v>
+      </c>
+      <c r="X70">
+        <v>13.05</v>
+      </c>
+      <c r="Y70">
+        <v>0</v>
+      </c>
+      <c r="Z70">
+        <v>1</v>
+      </c>
+      <c r="AA70">
+        <v>988</v>
+      </c>
+      <c r="AB70">
+        <v>50</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE70">
+        <v>0.1505667</v>
+      </c>
+      <c r="AF70">
+        <v>65</v>
+      </c>
+      <c r="AG70">
+        <v>1</v>
+      </c>
+      <c r="AH70">
+        <v>65</v>
+      </c>
+      <c r="AI70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71">
+        <v>1002</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>77.81</v>
+      </c>
+      <c r="H71" t="s">
+        <v>33</v>
+      </c>
+      <c r="I71" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71">
+        <v>60.01</v>
+      </c>
+      <c r="K71">
+        <v>9</v>
+      </c>
+      <c r="L71" t="s">
+        <v>35</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <v>7</v>
+      </c>
+      <c r="O71">
+        <v>781033223</v>
+      </c>
+      <c r="P71" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>37</v>
+      </c>
+      <c r="R71" t="s">
+        <v>37</v>
+      </c>
+      <c r="S71" s="1">
+        <v>43811</v>
+      </c>
+      <c r="U71" s="2">
+        <v>0.71615740740740741</v>
+      </c>
+      <c r="V71" t="s">
+        <v>38</v>
+      </c>
+      <c r="W71">
+        <v>66</v>
+      </c>
+      <c r="X71">
+        <v>10.53</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>1</v>
+      </c>
+      <c r="AA71">
+        <v>1060</v>
+      </c>
+      <c r="AB71">
+        <v>50</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE71">
+        <v>0.14610000000000001</v>
+      </c>
+      <c r="AF71">
+        <v>66</v>
+      </c>
+      <c r="AG71">
+        <v>1</v>
+      </c>
+      <c r="AH71">
+        <v>66</v>
+      </c>
+      <c r="AI71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>32</v>
+      </c>
+      <c r="E72">
+        <v>1002</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>77.81</v>
+      </c>
+      <c r="H72" t="s">
+        <v>33</v>
+      </c>
+      <c r="I72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72">
+        <v>60.01</v>
+      </c>
+      <c r="K72">
+        <v>9</v>
+      </c>
+      <c r="L72" t="s">
+        <v>35</v>
+      </c>
+      <c r="M72">
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <v>7</v>
+      </c>
+      <c r="O72">
+        <v>781033223</v>
+      </c>
+      <c r="P72" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>37</v>
+      </c>
+      <c r="R72" t="s">
+        <v>37</v>
+      </c>
+      <c r="S72" s="1">
+        <v>43811</v>
+      </c>
+      <c r="U72" s="2">
+        <v>0.71615740740740741</v>
+      </c>
+      <c r="V72" t="s">
+        <v>38</v>
+      </c>
+      <c r="W72">
+        <v>67</v>
+      </c>
+      <c r="X72">
+        <v>21.84</v>
+      </c>
+      <c r="Y72">
+        <v>1</v>
+      </c>
+      <c r="Z72">
+        <v>1</v>
+      </c>
+      <c r="AA72">
+        <v>1591</v>
+      </c>
+      <c r="AB72">
+        <v>88</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD72" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE72">
         <v>0.18381</v>
       </c>
-      <c r="AF68">
+      <c r="AF72">
         <v>67</v>
       </c>
-      <c r="AG68">
-        <v>1</v>
-      </c>
-      <c r="AH68">
+      <c r="AG72">
+        <v>1</v>
+      </c>
+      <c r="AH72">
         <v>67</v>
       </c>
-      <c r="AI68">
+      <c r="AI72">
         <v>21.84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
separated out data_mat into monetary and social matrices as well
</commit_message>
<xml_diff>
--- a/data/social/S_1002.xlsx
+++ b/data/social/S_1002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/social/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789D3C0-076C-0544-8716-2D282C986BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F809E5E1-4D3E-8C49-8D78-31E275236DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="42">
   <si>
     <t>ExperimentName</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Win</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -987,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1173,8 +1176,8 @@
       <c r="X2">
         <v>0</v>
       </c>
-      <c r="Y2">
-        <v>0</v>
+      <c r="Y2" t="s">
+        <v>41</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -1280,8 +1283,8 @@
       <c r="X3">
         <v>0</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
+      <c r="Y3" t="s">
+        <v>41</v>
       </c>
       <c r="Z3">
         <v>0</v>
@@ -1387,8 +1390,8 @@
       <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4">
-        <v>0</v>
+      <c r="Y4" t="s">
+        <v>41</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -1494,8 +1497,8 @@
       <c r="X5">
         <v>0</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
+      <c r="Y5" t="s">
+        <v>41</v>
       </c>
       <c r="Z5">
         <v>0</v>

</xml_diff>